<commit_message>
includes gauge length calculations
Former-commit-id: d774a02f92dbd51dc797cb71ffb0746b72d3eee5
</commit_message>
<xml_diff>
--- a/edd-tools/EDD_calculations_material.xlsx
+++ b/edd-tools/EDD_calculations_material.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parkjs\Documents\GitHub\matlab_tools\edd-tools\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="12900" yWindow="-15" windowWidth="15915" windowHeight="11640" activeTab="1"/>
   </bookViews>
@@ -13,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -24,7 +29,7 @@
     <author>parkjs</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1">
+    <comment ref="E1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -917,6 +922,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1290,8 +1298,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="158721152"/>
-        <c:axId val="158723072"/>
+        <c:axId val="242894432"/>
+        <c:axId val="243922520"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1627,11 +1635,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="159189632"/>
-        <c:axId val="159188096"/>
+        <c:axId val="243923304"/>
+        <c:axId val="243922912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="158721152"/>
+        <c:axId val="242894432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -1662,12 +1670,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158723072"/>
+        <c:crossAx val="243922520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="158723072"/>
+        <c:axId val="243922520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1699,12 +1707,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158721152"/>
+        <c:crossAx val="242894432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="159188096"/>
+        <c:axId val="243922912"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1716,12 +1724,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159189632"/>
+        <c:crossAx val="243923304"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="159189632"/>
+        <c:axId val="243923304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1731,7 +1739,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159188096"/>
+        <c:crossAx val="243922912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1785,415 +1793,6 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>bm_flux!$B$2:$B$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>155</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>165</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>175</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>235</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>250</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>bm_flux!$C$2:$C$51</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>15785700000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14919200000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13032300000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11027100000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9167920000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7536730000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6146850000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4983710000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4022090000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3233990000000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2592380000000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2072730000000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1653600000000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1316720000000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1046710000000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>830844000000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>658616000000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>521454000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>412387000000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>326015000000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>257400000000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>203063000000</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>160078000000</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>126106000000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>99281000000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>78116300000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>61429900000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>48283200000</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>37931800000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29786300000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>23380100000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>18344400000</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>14387900000</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>11280700000</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>8841610000</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>6927650000</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>5426370000</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4249210000</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3326490000</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2603470000</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2037080000</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1593530000</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1246280000</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>974481000</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>761799000</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>595416000</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>465282000</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>363523000</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>283968000</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>221785000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="159206400"/>
-        <c:axId val="159212288"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="159206400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159212288"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="159212288"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159206400"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
@@ -2831,11 +2430,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="159064448"/>
-        <c:axId val="159066368"/>
+        <c:axId val="243924088"/>
+        <c:axId val="243634800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="159064448"/>
+        <c:axId val="243924088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2864,12 +2463,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159066368"/>
+        <c:crossAx val="243634800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="159066368"/>
+        <c:axId val="243634800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -2913,7 +2512,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159064448"/>
+        <c:crossAx val="243924088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3018,36 +2617,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>862012</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3223,7 +2792,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3258,7 +2827,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3469,7 +3038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C51"/>
     </sheetView>
   </sheetViews>
@@ -4829,8 +4398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5010,11 +4579,11 @@
       </c>
       <c r="O5" s="19">
         <f>2*N5*SIN($C$16)</f>
-        <v>1.2102872298796554</v>
+        <v>0.52935982338689147</v>
       </c>
       <c r="P5" s="38">
         <f>$C$9/O5/1000*10000000000</f>
-        <v>10.244194493896728</v>
+        <v>23.421531496365745</v>
       </c>
       <c r="Q5" s="44"/>
       <c r="R5" s="45">
@@ -5067,11 +4636,11 @@
       </c>
       <c r="O6" s="19">
         <f t="shared" ref="O6:O33" si="3">2*N6*SIN($C$16)</f>
-        <v>1.0481394869516782</v>
+        <v>0.45843905479589181</v>
       </c>
       <c r="P6" s="38">
         <f t="shared" ref="P6:P33" si="4">$C$9/O6/1000*10000000000</f>
-        <v>11.828976897364315</v>
+        <v>27.044855028520121</v>
       </c>
       <c r="Q6" s="44"/>
       <c r="R6" s="45">
@@ -5124,11 +4693,11 @@
       </c>
       <c r="O7" s="19">
         <f t="shared" si="3"/>
-        <v>0.74114653885292037</v>
+        <v>0.32416536440692628</v>
       </c>
       <c r="P7" s="38">
         <f t="shared" si="4"/>
-        <v>16.728699557250632</v>
+        <v>38.247200773747366</v>
       </c>
       <c r="Q7" s="44"/>
       <c r="R7" s="45">
@@ -5181,11 +4750,11 @@
       </c>
       <c r="O8" s="19">
         <f t="shared" si="3"/>
-        <v>0.63205189203169565</v>
+        <v>0.27644915163693679</v>
       </c>
       <c r="P8" s="38">
         <f t="shared" si="4"/>
-        <v>19.616139011169899</v>
+        <v>44.848818319578868</v>
       </c>
       <c r="Q8" s="44"/>
       <c r="R8" s="45">
@@ -5232,11 +4801,11 @@
       </c>
       <c r="O9" s="19">
         <f t="shared" si="3"/>
-        <v>0.60514361493982771</v>
+        <v>0.26467991169344574</v>
       </c>
       <c r="P9" s="38">
         <f t="shared" si="4"/>
-        <v>20.488388987793456</v>
+        <v>46.84306299273149</v>
       </c>
       <c r="Q9" s="44"/>
       <c r="R9" s="45">
@@ -5276,11 +4845,11 @@
       </c>
       <c r="O10" s="19">
         <f t="shared" si="3"/>
-        <v>0.52406974347583912</v>
+        <v>0.2292195273979459</v>
       </c>
       <c r="P10" s="38">
         <f t="shared" si="4"/>
-        <v>23.65795379472863</v>
+        <v>54.089710057040243</v>
       </c>
       <c r="Q10" s="44"/>
       <c r="R10" s="45">
@@ -5328,11 +4897,11 @@
       </c>
       <c r="O11" s="19">
         <f t="shared" si="3"/>
-        <v>0.48091937919546662</v>
+        <v>0.21034626438185239</v>
       </c>
       <c r="P11" s="38">
         <f t="shared" si="4"/>
-        <v>25.780657450544176</v>
+        <v>58.942895006013522</v>
       </c>
       <c r="Q11" s="44"/>
       <c r="R11" s="45">
@@ -5378,11 +4947,11 @@
       </c>
       <c r="O12" s="19">
         <f t="shared" si="3"/>
-        <v>0.46874222854514119</v>
+        <v>0.20502017801287301</v>
       </c>
       <c r="P12" s="38">
         <f t="shared" si="4"/>
-        <v>26.450396446781159</v>
+        <v>60.474134285398016</v>
       </c>
       <c r="Q12" s="44"/>
       <c r="R12" s="45">
@@ -5422,11 +4991,11 @@
       </c>
       <c r="O13" s="19">
         <f t="shared" si="3"/>
-        <v>0.42790115371569309</v>
+        <v>0.18715696040229204</v>
       </c>
       <c r="P13" s="38">
         <f t="shared" si="4"/>
-        <v>28.974957577713067</v>
+        <v>66.24609498741809</v>
       </c>
       <c r="Q13" s="44"/>
       <c r="R13" s="45">
@@ -5444,7 +5013,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>2</v>
@@ -5472,11 +5041,11 @@
       </c>
       <c r="O14" s="19">
         <f t="shared" si="3"/>
-        <v>0.4034290766265517</v>
+        <v>0.17645327446229714</v>
       </c>
       <c r="P14" s="38">
         <f t="shared" si="4"/>
-        <v>30.732583481690185</v>
+        <v>70.264594489097249</v>
       </c>
       <c r="Q14" s="44"/>
       <c r="R14" s="45">
@@ -5495,7 +5064,7 @@
       </c>
       <c r="C15" s="1">
         <f>C14*PI()/180</f>
-        <v>0.52359877559829882</v>
+        <v>0.22689280275926285</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>4</v>
@@ -5524,11 +5093,11 @@
       </c>
       <c r="O15" s="19">
         <f t="shared" si="3"/>
-        <v>0.4034290766265517</v>
+        <v>0.17645327446229714</v>
       </c>
       <c r="P15" s="38">
         <f t="shared" si="4"/>
-        <v>30.732583481690185</v>
+        <v>70.264594489097249</v>
       </c>
       <c r="Q15" s="44"/>
       <c r="R15" s="45">
@@ -5547,7 +5116,7 @@
       </c>
       <c r="C16" s="1">
         <f>C15/2</f>
-        <v>0.26179938779914941</v>
+        <v>0.11344640137963143</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>4</v>
@@ -5576,11 +5145,11 @@
       </c>
       <c r="O16" s="19">
         <f t="shared" si="3"/>
-        <v>0.37057326942646018</v>
+        <v>0.16208268220346314</v>
       </c>
       <c r="P16" s="38">
         <f t="shared" si="4"/>
-        <v>33.457399114501264</v>
+        <v>76.494401547494732</v>
       </c>
       <c r="Q16" s="44"/>
       <c r="R16" s="45">
@@ -5621,11 +5190,11 @@
       </c>
       <c r="O17" s="19">
         <f t="shared" si="3"/>
-        <v>0.35433581877847015</v>
+        <v>0.154980687077787</v>
       </c>
       <c r="P17" s="38">
         <f t="shared" si="4"/>
-        <v>34.990585538624721</v>
+        <v>79.999760035543943</v>
       </c>
       <c r="Q17" s="44"/>
       <c r="R17" s="45">
@@ -5644,7 +5213,7 @@
       </c>
       <c r="C18" s="1">
         <f>$C$11*COS($C$16)/SIN($C$15)</f>
-        <v>0.19318516525781371</v>
+        <v>0.44168357359987842</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>0</v>
@@ -5672,11 +5241,11 @@
       </c>
       <c r="O18" s="19">
         <f t="shared" si="3"/>
-        <v>0.34937982898389269</v>
+        <v>0.15281301826529728</v>
       </c>
       <c r="P18" s="38">
         <f t="shared" si="4"/>
-        <v>35.486930692092947</v>
+        <v>81.134565085560368</v>
       </c>
       <c r="Q18" s="44"/>
       <c r="R18" s="45">
@@ -5695,7 +5264,7 @@
       </c>
       <c r="C19" s="1">
         <f>$C$12*COS($C$16)/SIN($C$15)</f>
-        <v>0.19318516525781371</v>
+        <v>0.44168357359987842</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>0</v>
@@ -5723,11 +5292,11 @@
       </c>
       <c r="O19" s="19">
         <f t="shared" si="3"/>
-        <v>0.34937982898389269</v>
+        <v>0.15281301826529728</v>
       </c>
       <c r="P19" s="38">
         <f t="shared" si="4"/>
-        <v>35.486930692092947</v>
+        <v>81.134565085560368</v>
       </c>
       <c r="Q19" s="44"/>
       <c r="R19" s="45">
@@ -5746,7 +5315,7 @@
       </c>
       <c r="C20" s="1">
         <f>C19+C18</f>
-        <v>0.38637033051562741</v>
+        <v>0.88336714719975684</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>0</v>
@@ -5774,11 +5343,11 @@
       </c>
       <c r="O20" s="19">
         <f t="shared" si="3"/>
-        <v>0.33145080843276381</v>
+        <v>0.14497115815297559</v>
       </c>
       <c r="P20" s="38">
         <f t="shared" si="4"/>
-        <v>37.406509385183043</v>
+        <v>85.523340879181674</v>
       </c>
       <c r="Q20" s="44"/>
       <c r="R20" s="45">
@@ -5818,11 +5387,11 @@
       </c>
       <c r="O21" s="19">
         <f t="shared" si="3"/>
-        <v>0.31967954653856134</v>
+        <v>0.13982260088200824</v>
       </c>
       <c r="P21" s="38">
         <f t="shared" si="4"/>
-        <v>38.783894404927551</v>
+        <v>88.672487124090253</v>
       </c>
       <c r="Q21" s="44"/>
       <c r="R21" s="45">
@@ -5841,7 +5410,7 @@
       </c>
       <c r="C22" s="1">
         <f>$C$11*SIN($C$16)/SIN($C$15)</f>
-        <v>5.1763809020504155E-2</v>
+        <v>5.0323486634946762E-2</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>0</v>
@@ -5869,11 +5438,11 @@
       </c>
       <c r="O22" s="19">
         <f t="shared" si="3"/>
-        <v>0.31602594601584783</v>
+        <v>0.13822457581846839</v>
       </c>
       <c r="P22" s="38">
         <f t="shared" si="4"/>
-        <v>39.232278022339798</v>
+        <v>89.697636639157736</v>
       </c>
       <c r="Q22" s="44"/>
       <c r="R22" s="45">
@@ -5892,7 +5461,7 @@
       </c>
       <c r="C23" s="1">
         <f>$C$12*SIN($C$16)/SIN($C$15)</f>
-        <v>5.1763809020504155E-2</v>
+        <v>5.0323486634946762E-2</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>0</v>
@@ -5920,11 +5489,11 @@
       </c>
       <c r="O23" s="19">
         <f t="shared" si="3"/>
-        <v>0.30257180746991386</v>
+        <v>0.13233995584672287</v>
       </c>
       <c r="P23" s="38">
         <f t="shared" si="4"/>
-        <v>40.976777975586913</v>
+        <v>93.686125985462979</v>
       </c>
       <c r="Q23" s="44"/>
       <c r="R23" s="45">
@@ -5943,7 +5512,7 @@
       </c>
       <c r="C24" s="1">
         <f>C22+C23</f>
-        <v>0.10352761804100831</v>
+        <v>0.10064697326989352</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>0</v>
@@ -5971,11 +5540,11 @@
       </c>
       <c r="O24" s="19">
         <f t="shared" si="3"/>
-        <v>0.29353776977235418</v>
+        <v>0.12838861563426254</v>
       </c>
       <c r="P24" s="38">
         <f t="shared" si="4"/>
-        <v>42.237895947707059</v>
+        <v>96.569448273246834</v>
       </c>
       <c r="Q24" s="44"/>
       <c r="R24" s="45">
@@ -6012,11 +5581,11 @@
       </c>
       <c r="O25" s="19">
         <f t="shared" si="3"/>
-        <v>0.29353776977235418</v>
+        <v>0.12838861563426254</v>
       </c>
       <c r="P25" s="38">
         <f t="shared" si="4"/>
-        <v>42.237895947707059</v>
+        <v>96.569448273246834</v>
       </c>
       <c r="Q25" s="44"/>
       <c r="R25" s="45">
@@ -6056,11 +5625,11 @@
       </c>
       <c r="O26" s="19">
         <f t="shared" si="3"/>
-        <v>0.2907015895417534</v>
+        <v>0.12714811682629487</v>
       </c>
       <c r="P26" s="38">
         <f t="shared" si="4"/>
-        <v>42.649982739725985</v>
+        <v>97.511611542819438</v>
       </c>
       <c r="Q26" s="44"/>
       <c r="R26" s="45">
@@ -6097,11 +5666,11 @@
       </c>
       <c r="O27" s="19">
         <f t="shared" si="3"/>
-        <v>0.28012706098015683</v>
+        <v>0.12252299112590803</v>
       </c>
       <c r="P27" s="38">
         <f t="shared" si="4"/>
-        <v>44.25997878600149</v>
+        <v>101.19258159169267</v>
       </c>
       <c r="Q27" s="44"/>
       <c r="R27" s="45">
@@ -6138,11 +5707,11 @@
       </c>
       <c r="O28" s="19">
         <f t="shared" si="3"/>
-        <v>0.27291227672447682</v>
+        <v>0.11936736258991078</v>
       </c>
       <c r="P28" s="38">
         <f t="shared" si="4"/>
-        <v>45.430047798412964</v>
+        <v>103.86773660202016</v>
       </c>
       <c r="Q28" s="44"/>
       <c r="R28" s="45">
@@ -6179,11 +5748,11 @@
       </c>
       <c r="O29" s="19">
         <f t="shared" si="3"/>
-        <v>0.27291227672447682</v>
+        <v>0.11936736258991078</v>
       </c>
       <c r="P29" s="38">
         <f t="shared" si="4"/>
-        <v>45.430047798412964</v>
+        <v>103.86773660202016</v>
       </c>
       <c r="Q29" s="44"/>
       <c r="R29" s="45">
@@ -6220,11 +5789,11 @@
       </c>
       <c r="O30" s="19">
         <f t="shared" si="3"/>
-        <v>0.26203487173791956</v>
+        <v>0.11460976369897295</v>
       </c>
       <c r="P30" s="38">
         <f t="shared" si="4"/>
-        <v>47.315907589457261</v>
+        <v>108.17942011408049</v>
       </c>
       <c r="Q30" s="44"/>
       <c r="R30" s="45">
@@ -6261,11 +5830,11 @@
       </c>
       <c r="O31" s="19">
         <f t="shared" si="3"/>
-        <v>0.25610123745757868</v>
+        <v>0.11201448919128772</v>
       </c>
       <c r="P31" s="38">
         <f t="shared" si="4"/>
-        <v>48.412174417628087</v>
+        <v>110.6858395362929</v>
       </c>
       <c r="Q31" s="44"/>
       <c r="R31" s="45">
@@ -6302,11 +5871,11 @@
       </c>
       <c r="O32" s="19">
         <f t="shared" si="3"/>
-        <v>0.25421116559308665</v>
+        <v>0.11118780269598733</v>
       </c>
       <c r="P32" s="38">
         <f t="shared" si="4"/>
-        <v>48.772121190824151</v>
+        <v>111.5087939121054</v>
       </c>
       <c r="Q32" s="44"/>
       <c r="R32" s="45">
@@ -6345,11 +5914,11 @@
       </c>
       <c r="O33" s="19">
         <f t="shared" si="3"/>
-        <v>0.25421116559308665</v>
+        <v>0.11118780269598733</v>
       </c>
       <c r="P33" s="38">
         <f t="shared" si="4"/>
-        <v>48.772121190824151</v>
+        <v>111.5087939121054</v>
       </c>
       <c r="Q33" s="44"/>
       <c r="R33" s="45">

</xml_diff>